<commit_message>
Worked on the Month function
</commit_message>
<xml_diff>
--- a/CH-163 Custom Grouping.xlsx
+++ b/CH-163 Custom Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CD8B16-8F11-4A7B-8142-1934ED1C1D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB81F83-8082-4142-8411-94FA128E6FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,10 +17,22 @@
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_fBCAST">_xlfn.LAMBDA(_xlpm._nData, _xlfn.LET(_xlpm.f, _xlfn.LAMBDA(_xlpm._d, _xlfn.LET(_xlpm._c, COLUMNS(_xlpm._d) - 1, _xlfn.DROP(_xlfn.REDUCE("", _xlfn.TAKE(_xlpm._d, , 1), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.VSTACK(_xlpm.a, _xlfn.EXPAND(_xlpm.v, _xlpm._c, 1, _xlpm.v)))), 1))), _xlfn.HSTACK(_xlpm.f(_xlpm._nData), _xlfn.TOCOL(_xlfn.DROP(_xlpm._nData, , 1)))))</definedName>
+    <definedName name="_fCharCount">_xlfn.LAMBDA(_xlpm.s,_xlpm.c, _xlfn.LET(_xlpm.z, SUBSTITUTE(_xlpm.s, _xlpm.c, ""), LEN(_xlpm.s) - LEN(_xlpm.z)))</definedName>
+    <definedName name="_fDN">_xlfn.LAMBDA(_xlpm.arr,_xlop.ini, _xlfn.LET(_xlpm._ini, IF(_xlfn.ISOMITTED(_xlpm.ini), "", _xlpm.ini), _xlfn.SCAN(_xlpm._ini, _xlpm.arr, _xlfn.LAMBDA(_xlpm.a,_xlpm.v, IF(LEN(_xlpm.v) = 0, _xlpm.a, _xlpm.v)))))</definedName>
+    <definedName name="_fDX">_xlfn.LAMBDA(_xlpm.vlookup_value,_xlpm.vlookup_array,_xlpm.hlookup_value,_xlpm.hlookup_array,_xlpm.return_array,_xlop.if_not_found,_xlop.vmatch_mode,_xlop.vsearch_mode,_xlop.hmatch_mode,_xlop.hsearch_mode, IFERROR(INDEX(_xlpm.return_array, _xlfn.XMATCH(_xlpm.vlookup_value, _xlpm.vlookup_array, _xlpm.vmatch_mode, _xlpm.vsearch_mode), _xlfn.XMATCH(_xlpm.hlookup_value, _xlpm.hlookup_array, _xlpm.hmatch_mode, _xlpm.hsearch_mode)), IF(ISOMlTTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found)))</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$D$23</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$23</definedName>
+    <definedName name="_fIndex">_xlfn.LAMBDA(_xlpm.d,_xlpm.r, INDEX(_xlpm.d, _xlpm.r, _xlfn.SEQUENCE(1, COLUMNS(_xlpm.d))))</definedName>
+    <definedName name="_fInterp">_xlfn.LAMBDA(_xlpm.x,_xlpm.xdat,_xlpm.ydat, _xlfn.LET(_xlpm.xmin, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.xdat, , -1), _xlpm.xmax, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.xdat, , 1), _xlpm.ymin, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.ydat, , -1), _xlpm.ymax, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.ydat, , 1), IF(_xlpm.xmin = _xlpm.xmax, _xlpm.ymin, (_xlpm.ymin * (_xlpm.xmax - _xlpm.x) + _xlpm.ymax * (_xlpm.x - _xlpm.xmin)) / (_xlpm.xmax - _xlpm.xmin))))</definedName>
+    <definedName name="_fQ">_xlfn.LAMBDA(_xlpm.x, ROUNDUP(MONTH(1 &amp; _xlpm.x) / 3, 0))</definedName>
+    <definedName name="_fSUPERXLOOKUP">_xlfn.LAMBDA(_xlpm.lookup_value,_xlpm.lookup_array,_xlpm.return_array,_xlop.if_not_found,_xlop.match_mode,_xlop.search_mode, IF(COLUMNS(_xlpm.lookup_value) = 1, IFERROR(INDEX(_xlpm.return_array, _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode), _xlfn.SEQUENCE(1, COLUMNS(_xlpm.return_array))), IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found)), IFERROR(INDEX(_xlpm.return_array, _xlfn.SEQUENCE(ROWS(_xlpm.return_array)), _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode)), IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found))))</definedName>
+    <definedName name="_fUP">_xlfn.LAMBDA(_xlpm.arr,_xlop.ini, _xlfn.LET(_xlpm._f, _xlfn.LAMBDA(_xlpm.z, INDEX(_xlpm.z, _xlfn.SEQUENCE(ROWS(_xlpm.z), 1, ROWS(_xlpm.z), -1))), _xlpm._arr, _xlpm._f(_xlpm.arr), _xlpm._ini, IF(_xlfn.ISOMITTED(_xlpm.ini), "", _xlpm.ini), _xlpm._f(_xlfn.SCAN(_xlpm._ini, _xlpm._arr, _xlfn.LAMBDA(_xlpm.a,_xlpm.v, IF(LEN(_xlpm.v) = 0, _xlpm.a, _xlpm.v))))))</definedName>
+    <definedName name="DDL">_xlfn.LAMBDA(_xlpm.range,_xlop.lookup1,_xlop.lookup2,_xlop.lookup3,_xlop.lookup4,_xlop.lookup5,_xlop.lookup6,_xlop.lookup7,_xlop.lookup8,_xlop.lookup9,_xlop.lookup10, _xlfn.LET(_xlpm._s, "%^&amp;&amp;@", _xlpm.lookupValue, _xlpm.lookup1 &amp; _xlpm._s &amp; _xlpm.lookup2 &amp; _xlpm._s &amp; _xlpm.lookup3 &amp; _xlpm._s &amp; _xlpm.lookup4 &amp; _xlpm._s &amp; _xlpm.lookup5 &amp; _xlpm._s &amp; _xlpm.lookup6 &amp; _xlpm._s &amp; _xlpm.lookup7 &amp; _xlpm._s &amp; _xlpm.lookup8 &amp; _xlpm._s &amp; _xlpm.lookup9 &amp; _xlpm._s &amp; _xlpm.lookup10, _xlpm.levelIndex, IFERROR(ROWS(_xlfn.TEXTSPLIT(_xlpm.lookupValue, , _xlpm._s, TRUE())), 0) + 1, _xlpm.lookupArray, _xlfn.BYROW(_xlfn.EXPAND(_xlfn.CHOOSECOLS(_xlpm.range, _xlfn.SEQUENCE(1, _xlpm.levelIndex - 1)), , 10, ""), _xlfn.LAMBDA(_xlpm.row, _xlfn.TEXTJOIN(_xlpm._s, FALSE, _xlpm.row))), _xlpm.returnRange, INDEX(_xlpm.range, 0, _xlpm.levelIndex), _xlpm.result, IF(_xlfn.ISOMITTED(_xlpm.lookup1) * _xlpm.levelIndex = 1, _xlpm.returnRange, _xlfn.XLOOKUP(_xlpm.lookupValue, _xlpm.lookupArray, _xlpm.returnRange):_xlfn.XLOOKUP(_xlpm.lookupValue, _xlpm.lookupArray, _xlpm.returnRange, , , -1)), _xlpm.result))</definedName>
+    <definedName name="DDLSorter">_xlfn.LAMBDA(_xlpm.Range,_xlop.SortOrder, _xlfn._xlws.SORT(_xlpm.Range, _xlfn.SEQUENCE(, COLUMNS(_xlpm.Range)), _xlpm.SortOrder))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -63,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="21">
   <si>
     <t>Question</t>
   </si>
@@ -124,6 +136,9 @@
   <si>
     <t>https://www.linkedin.com/in/omid-motamedisedeh-74aba166/recent-activity/all/</t>
   </si>
+  <si>
+    <t>ROUNDUP(MONTH(--(1 &amp; C3:C39)) / 3, 0)</t>
+  </si>
 </sst>
 </file>
 
@@ -132,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;\-0;0;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +173,14 @@
       <color theme="1"/>
       <name val="Corbel"/>
       <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Corbel"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -294,10 +317,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -360,15 +384,22 @@
     <xf numFmtId="3" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -977,7 +1008,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="892" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="976" row="9">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -989,10 +1020,15 @@
   <we:alternateReferences>
     <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
   </we:alternateReferences>
-  <we:properties/>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{30971B20-B398-44D5-A36C-AF779314A9EE}&quot;}"/>
+  </we:properties>
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1022,17 +1058,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
       <c r="E1"/>
-      <c r="G1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
+      <c r="G1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
       <c r="K1" s="6" t="s">
         <v>19</v>
       </c>
@@ -1679,10 +1715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F410690E-D8D2-49EA-83E7-40BEABC931DF}">
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:N90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1698,17 +1734,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
       <c r="E1"/>
-      <c r="G1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
+      <c r="G1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
       <c r="K1" s="6" t="s">
         <v>19</v>
       </c>
@@ -1762,7 +1798,7 @@
       <c r="L3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="26">
+      <c r="M3" s="24">
         <v>1</v>
       </c>
     </row>
@@ -1793,7 +1829,7 @@
       <c r="L4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="26">
+      <c r="M4" s="24">
         <v>1</v>
       </c>
     </row>
@@ -1824,7 +1860,7 @@
       <c r="L5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="26">
+      <c r="M5" s="24">
         <v>1</v>
       </c>
     </row>
@@ -1855,7 +1891,7 @@
       <c r="L6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="26">
+      <c r="M6" s="24">
         <v>2</v>
       </c>
     </row>
@@ -1884,7 +1920,7 @@
       <c r="L7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="26">
+      <c r="M7" s="24">
         <v>2</v>
       </c>
     </row>
@@ -1916,7 +1952,7 @@
       <c r="L8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="26">
+      <c r="M8" s="24">
         <v>2</v>
       </c>
     </row>
@@ -1948,7 +1984,7 @@
       <c r="L9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="26">
+      <c r="M9" s="24">
         <v>3</v>
       </c>
     </row>
@@ -1980,7 +2016,7 @@
       <c r="L10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="26">
+      <c r="M10" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2012,7 +2048,7 @@
       <c r="L11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="26">
+      <c r="M11" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2044,7 +2080,7 @@
       <c r="L12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M12" s="26">
+      <c r="M12" s="24">
         <v>4</v>
       </c>
       <c r="N12"/>
@@ -2074,7 +2110,7 @@
       <c r="L13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M13" s="26">
+      <c r="M13" s="24">
         <v>4</v>
       </c>
     </row>
@@ -2103,7 +2139,7 @@
       <c r="L14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M14" s="26">
+      <c r="M14" s="24">
         <v>4</v>
       </c>
     </row>
@@ -2869,6 +2905,9 @@
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B43" s="27" t="s">
+        <v>20</v>
+      </c>
       <c r="G43" s="4">
         <v>2021</v>
       </c>
@@ -2909,6 +2948,26 @@
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B45" s="3" t="str" cm="1">
+        <f t="array" ref="B45:B81">1&amp;C3:C39</f>
+        <v>1Jan</v>
+      </c>
+      <c r="C45" cm="1">
+        <f t="array" ref="C45:C81">MONTH(_xlfn.ANCHORARRAY(B45))/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D45">
+        <f>ROUNDUP(C45,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E45" cm="1">
+        <f t="array" ref="E45:E81">_fQ(C3:C39)</f>
+        <v>1</v>
+      </c>
+      <c r="F45" t="b" cm="1">
+        <f t="array" ref="F45:F82">D45:D82=_xlfn.ANCHORARRAY(E45)</f>
+        <v>1</v>
+      </c>
       <c r="G45" s="4">
         <v>2021</v>
       </c>
@@ -2929,6 +2988,22 @@
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B46" s="3" t="str">
+        <v>1Feb</v>
+      </c>
+      <c r="C46">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D46">
+        <f t="shared" ref="D46:D81" si="0">ROUNDUP(C46,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" t="b">
+        <v>1</v>
+      </c>
       <c r="G46" s="4">
         <v>2022</v>
       </c>
@@ -2949,6 +3024,22 @@
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B47" s="3" t="str">
+        <v>1Mar</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
       <c r="G47" s="4">
         <v>2022</v>
       </c>
@@ -2969,6 +3060,22 @@
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B48" s="3" t="str">
+        <v>1Apr</v>
+      </c>
+      <c r="C48">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
       <c r="G48" s="4">
         <v>2022</v>
       </c>
@@ -2988,7 +3095,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B49" s="3" t="str">
+        <v>1May</v>
+      </c>
+      <c r="C49">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
       <c r="G49" s="4">
         <v>2022</v>
       </c>
@@ -3008,7 +3131,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B50" s="3" t="str">
+        <v>1Jul</v>
+      </c>
+      <c r="C50">
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
       <c r="G50" s="4">
         <v>2023</v>
       </c>
@@ -3028,7 +3167,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B51" s="3" t="str">
+        <v>1Aug</v>
+      </c>
+      <c r="C51">
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
       <c r="G51" s="4">
         <v>2023</v>
       </c>
@@ -3048,7 +3203,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B52" s="3" t="str">
+        <v>1Sep</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
       <c r="G52" s="4">
         <v>2023</v>
       </c>
@@ -3066,6 +3237,572 @@
       </c>
       <c r="M52" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B53" s="3" t="str">
+        <v>1Oct</v>
+      </c>
+      <c r="C53">
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E53">
+        <v>4</v>
+      </c>
+      <c r="F53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B54" s="3" t="str">
+        <v>1Nov</v>
+      </c>
+      <c r="C54">
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B55" s="3" t="str">
+        <v>1Dec</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E55">
+        <v>4</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B56" s="3" t="str">
+        <v>1Feb</v>
+      </c>
+      <c r="C56">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B57" s="3" t="str">
+        <v>1Mar</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B58" s="3" t="str">
+        <v>1Apr</v>
+      </c>
+      <c r="C58">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B59" s="3" t="str">
+        <v>1May</v>
+      </c>
+      <c r="C59">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B60" s="3" t="str">
+        <v>1Jun</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B61" s="3" t="str">
+        <v>1Jul</v>
+      </c>
+      <c r="C61">
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+      <c r="F61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B62" s="3" t="str">
+        <v>1Aug</v>
+      </c>
+      <c r="C62">
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="F62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B63" s="3" t="str">
+        <v>1Sep</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="F63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B64" s="3" t="str">
+        <v>1Oct</v>
+      </c>
+      <c r="C64">
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E64">
+        <v>4</v>
+      </c>
+      <c r="F64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B65" s="3" t="str">
+        <v>1Nov</v>
+      </c>
+      <c r="C65">
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E65">
+        <v>4</v>
+      </c>
+      <c r="F65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B66" s="3" t="str">
+        <v>1Jan</v>
+      </c>
+      <c r="C66">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B67" s="3" t="str">
+        <v>1Feb</v>
+      </c>
+      <c r="C67">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B68" s="3" t="str">
+        <v>1Mar</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B69" s="3" t="str">
+        <v>1Apr</v>
+      </c>
+      <c r="C69">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
+      <c r="F69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B70" s="3" t="str">
+        <v>1May</v>
+      </c>
+      <c r="C70">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="F70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B71" s="3" t="str">
+        <v>1Jun</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E71">
+        <v>2</v>
+      </c>
+      <c r="F71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B72" s="3" t="str">
+        <v>1Jul</v>
+      </c>
+      <c r="C72">
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E72">
+        <v>3</v>
+      </c>
+      <c r="F72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B73" s="3" t="str">
+        <v>1Aug</v>
+      </c>
+      <c r="C73">
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E73">
+        <v>3</v>
+      </c>
+      <c r="F73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B74" s="3" t="str">
+        <v>1Sep</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E74">
+        <v>3</v>
+      </c>
+      <c r="F74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B75" s="3" t="str">
+        <v>1Oct</v>
+      </c>
+      <c r="C75">
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E75">
+        <v>4</v>
+      </c>
+      <c r="F75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B76" s="3" t="str">
+        <v>1Dec</v>
+      </c>
+      <c r="C76">
+        <v>4</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E76">
+        <v>4</v>
+      </c>
+      <c r="F76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B77" s="3" t="str">
+        <v>1Feb</v>
+      </c>
+      <c r="C77">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B78" s="3" t="str">
+        <v>1Mar</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B79" s="3" t="str">
+        <v>1Apr</v>
+      </c>
+      <c r="C79">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
+      <c r="F79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B80" s="3" t="str">
+        <v>1Jun</v>
+      </c>
+      <c r="C80">
+        <v>2</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="F80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B81" s="3" t="str">
+        <v>1Jul</v>
+      </c>
+      <c r="C81">
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E81">
+        <v>3</v>
+      </c>
+      <c r="F81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F82" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B84" s="28"/>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B85" s="3" cm="1">
+        <f t="array" ref="B85">_xlfn.LAMBDA(_xlpm.x,ROUNDUP(MONTH(1&amp;_xlpm.x)/3,0))(C4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B86" s="3" cm="1">
+        <f t="array" ref="B86">_xlfn.LAMBDA(_xlpm.x,ROUNDUP(MONTH(1&amp;_xlpm.x)/3,0))(C5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B87" s="3" cm="1">
+        <f t="array" ref="B87">_xlfn.LAMBDA(_xlpm.x,ROUNDUP(MONTH(1&amp;_xlpm.x)/3,0))(C6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B88" s="3" cm="1">
+        <f t="array" ref="B88">_xlfn.LAMBDA(_xlpm.x,ROUNDUP(MONTH(1&amp;_xlpm.x)/3,0))(C7)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B89" s="3" cm="1">
+        <f t="array" ref="B89">_xlfn.LAMBDA(_xlpm.x,ROUNDUP(MONTH(1&amp;_xlpm.x)/3,0))(C8)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B90" s="3" cm="1">
+        <f t="array" ref="B90">_xlfn.LAMBDA(_xlpm.x,ROUNDUP(MONTH(1&amp;_xlpm.x)/3,0))(C9)</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3077,4 +3814,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIABHAGUAbgBlAHIAYQB0AGUAIABhAG4AIABpAG4AZABlAHgAIABjAG8AbAB1AG0AbgAgAHQAaABlACAAaABlAGkAZwBoAHQAIABvAGYAIAB0AGgAZQAgAGQAYQB0AGEAIABkAFwAbgBfAGYASQBuAGQAZQB4AD0ATABBAE0AQgBEAEEAKABkACwAcgAsAEkATgBEAEUAWAAoAGQALAByACwAUwBFAFEAVQBFAE4AQwBFACgAMQAsAEMATwBMAFUATQBOAFMAKABkACkAKQApACkAOwBcAG4ALwAvACAAUwB1AHAAZQByAFgATABPAE8ASwBVAFAAXABuAF8AZgBTAFUAUABFAFIAWABMAE8ATwBLAFUAUAA9AEwAQQBNAEIARABBACgAbABvAG8AawB1AHAAXwB2AGEAbAB1AGUALABsAG8AbwBrAHUAcABfAGEAcgByAGEAeQAsAHIAZQB0AHUAcgBuAF8AYQByAHIAYQB5ACwAWwBpAGYAXwBuAG8AdABfAGYAbwB1AG4AZABdACwAWwBtAGEAdABjAGgAXwBtAG8AZABlAF0ALABbAHMAZQBhAHIAYwBoAF8AbQBvAGQAZQBdACwAXABuACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIABDAE8ATABVAE0ATgBTACgAbABvAG8AawB1AHAAXwB2AGEAbAB1AGUAKQAgAD0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIABJAEYARQBSAFIATwBSACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHIAZQB0AHUAcgBuAF8AYQByAHIAYQB5ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAWABNAEEAVABDAEgAKABsAG8AbwBrAHUAcABfAHYAYQBsAHUAZQAsACAAbABvAG8AawB1AHAAXwBhAHIAcgBhAHkALAAgAG0AYQB0AGMAaABfAG0AbwBkAGUALAAgAHMAZQBhAHIAYwBoAF8AbQBvAGQAZQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUwBFAFEAVQBFAE4AQwBFACgAMQAsACAAQwBPAEwAVQBNAE4AUwAoAHIAZQB0AHUAcgBuAF8AYQByAHIAYQB5ACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGkAZgBfAG4AbwB0AF8AZgBvAHUAbgBkACkALAAgAE4AQQAoACkALAAgAGkAZgBfAG4AbwB0AF8AZgBvAHUAbgBkACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABJAEYARQBSAFIATwBSACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHIAZQB0AHUAcgBuAF8AYQByAHIAYQB5ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUwBFAFEAVQBFAE4AQwBFACgAUgBPAFcAUwAoAHIAZQB0AHUAcgBuAF8AYQByAHIAYQB5ACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFgATQBBAFQAQwBIACgAbABvAG8AawB1AHAAXwB2AGEAbAB1AGUALAAgAGwAbwBvAGsAdQBwAF8AYQByAHIAYQB5ACwAIABtAGEAdABjAGgAXwBtAG8AZABlACwAIABzAGUAYQByAGMAaABfAG0AbwBkAGUAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGkAZgBfAG4AbwB0AF8AZgBvAHUAbgBkACkALAAgAE4AQQAoACkALAAgAGkAZgBfAG4AbwB0AF8AZgBvAHUAbgBkACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8ALwAgAEwAaQBuAGUAYQByACAASQBuAHQAZQByAHAAbwBsAGEAdABpAG8AbgAgAEYAbwByAG0AdQBsAGEAXABuAF8AZgBJAG4AdABlAHIAcAA9AEwAQQBNAEIARABBACgAeAAsAHgAZABhAHQALAB5AGQAYQB0ACwAXABuACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAB4AG0AaQBuACwAIABYAEwATwBPAEsAVQBQACgAeAAsAHgAZABhAHQALAB4AGQAYQB0ACwALAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAB4AG0AYQB4ACwAIABYAEwATwBPAEsAVQBQACgAeAAsAHgAZABhAHQALAB4AGQAYQB0ACwALAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAeQBtAGkAbgAsACAAWABMAE8ATwBLAFUAUAAoAHgALAB4AGQAYQB0ACwAeQBkAGEAdAAsACwALQAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAeQBtAGEAeAAsACAAWABMAE8ATwBLAFUAUAAoAHgALAB4AGQAYQB0ACwAeQBkAGEAdAAsACwAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgAEkARgAoAHgAbQBpAG4APQB4AG0AYQB4ACwAeQBtAGkAbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAHkAbQBpAG4AKgAoAHgAbQBhAHgALQB4ACkAKwB5AG0AYQB4ACoAKAB4AC0AeABtAGkAbgApACkALwAoAHgAbQBhAHgALQB4AG0AaQBuACkAKQBcAG4AIAAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8ALwAgAEMAbwB1AG4AdAAgAGEAIABzAHAAZQBjAGkAZgBpAGMAIABjAGgAYQByAGEAYwB0AGUAcgAgAGkAbgAgAGEAIABzAHQAcgBpAG4AZwBcAG4AXwBmAEMAaABhAHIAQwBvAHUAbgB0AD0ATABBAE0AQgBEAEEAKABzACwAYwAsAEwARQBUACgAegAsAFMAVQBCAFMAVABJAFQAVQBUAEUAKABzACwAYwAsAFwAIgBcACIAKQAsAEwARQBOACgAcwApAC0ATABFAE4AKAB6ACkAKQApADsAXABuAFwAbgAvAC8AIABGAGkAbABsACAARABvAHcAbgBcAG4AXwBmAEQATgA9AEwAQQBNAEIARABBACgAYQByAHIALABbAGkAbgBpAF0ALABcAG4ATABFAFQAKABcAG4AXwBpAG4AaQAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABpAG4AaQApACwAXAAiAFwAIgAsAGkAbgBpACkALABcAG4AUwBDAEEATgAoAF8AaQBuAGkALABhAHIAcgAsAEwAQQBNAEIARABBACgAYQAsAHYALABJAEYAKABMAEUATgAoAHYAKQA9ADAALABhACwAdgApACkAKQBcAG4AKQBcAG4AKQA7AFwAbgBcAG4ALwAvACAARgBpAGwAbAAgAFUAcABcAG4AXwBmAFUAUAA9AEwAQQBNAEIARABBACgAYQByAHIALABbAGkAbgBpAF0ALABcAG4ATABFAFQAKABcAG4AXwBmACwATABBAE0AQgBEAEEAKAB6ACwASQBOAEQARQBYACgAegAsAFMARQBRAFUARQBOAEMARQAoAFIATwBXAFMAKAB6ACkALAAxACwAUgBPAFcAUwAoAHoAKQAsAC0AMQApACkAKQAsAFwAbgBfAGEAcgByACwAIABfAGYAKABhAHIAcgApACwAXABuAF8AaQBuAGkALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAaQBuAGkAKQAsAFwAIgBcACIALABpAG4AaQApACwAXABuAF8AZgAoAFMAQwBBAE4AKABfAGkAbgBpACwAXwBhAHIAcgAsAEwAQQBNAEIARABBACgAYQAsAHYALABJAEYAKABMAEUATgAoAHYAKQA9ADAALABhACwAdgApACkAKQApAFwAbgApAFwAbgApADsAXABuAFwAbgAvAC8AIABCAHIAbwBhAGQAYwBhAHMAdAAgAGYAaQByAHMAdAAgAGMAbwBsAHUAbQBuAFwAbgBfAGYAQgBDAEEAUwBUAD0ATABBAE0AQgBEAEEAKABfAG4ARABhAHQAYQAsAEwARQBUACgAZgAsACAATABBAE0AQgBEAEEAKABfAGQALABMAEUAVAAoAF8AYwAsAEMATwBMAFUATQBOAFMAKABfAGQAKQAtADEALABEAFIATwBQACgAUgBFAEQAVQBDAEUAKABcACIAXAAiACwAVABBAEsARQAoAF8AZAAsACwAMQApACwATABBAE0AQgBEAEEAKABhACwAdgAsAFYAUwBUAEEAQwBLACgAYQAsAEUAWABQAEEATgBEACgAdgAsAF8AYwAsADEALAB2ACkAKQApACkALAAxACkAKQApACwAXABuACAAIAAgACAAIABIAFMAVABBAEMASwAoAGYAKABfAG4ARABhAHQAYQApACwAVABPAEMATwBMACgARABSAE8AUAAoAF8AbgBEAGEAdABhACwALAAxACkAKQApAFwAbgApACkAOwBcAG4AXABuAC8ALwAgAE0AYQByAGsAIABQAHIAbwBjAHQAbwByACAARABEAEwAIABmAHUAbgBjAHQAaQBvAG4AXABuAEQARABMAD0ATABBAE0AQgBEAEEAKAByAGEAbgBnAGUALABbAGwAbwBvAGsAdQBwADEAXQAsAFsAbABvAG8AawB1AHAAMgBdACwAWwBsAG8AbwBrAHUAcAAzAF0ALABbAGwAbwBvAGsAdQBwADQAXQAsAFsAbABvAG8AawB1AHAANQBdACwAWwBsAG8AbwBrAHUAcAA2AF0ALABbAGwAbwBvAGsAdQBwADcAXQAsAFsAbABvAG8AawB1AHAAOABdACwAWwBsAG8AbwBrAHUAcAA5AF0ALABbAGwAbwBvAGsAdQBwADEAMABdACwAXABuAEwARQBUACgAXABuAF8AcwAsACAAXAAiACUAXgAmACYAQABcACIALAAgAFwAbgBsAG8AbwBrAHUAcABWAGEAbAB1AGUALAAgAGwAbwBvAGsAdQBwADEAIAAmACAAXwBzACAAJgAgAGwAbwBvAGsAdQBwADIAIAAmACAAXwBzACAAJgAgAGwAbwBvAGsAdQBwADMAIAAmACAAXwBzACAAJgAgAGwAbwBvAGsAdQBwADQAIAAmACAAXwBzACAAJgAgAGwAbwBvAGsAdQBwADUAIAAmACAAXwBzACAAJgAgAGwAbwBvAGsAdQBwADYAIAAmACAAXwBzACAAJgAgAGwAbwBvAGsAdQBwADcAIAAmACAAXwBzACAAJgAgAGwAbwBvAGsAdQBwADgAIAAmACAAXwBzACAAJgAgAGwAbwBvAGsAdQBwADkAIAAmACAAXwBzACAAJgAgAGwAbwBvAGsAdQBwADEAMAAsAFwAbgBsAGUAdgBlAGwASQBuAGQAZQB4ACwAIABJAEYARQBSAFIATwBSACgAUgBPAFcAUwAoAFQARQBYAFQAUwBQAEwASQBUACgAbABvAG8AawB1AHAAVgBhAGwAdQBlACwAIAAsACAAXwBzACwAIABUAFIAVQBFACgAKQApACkALAAgADAAKQAgACsAIAAxACwAIABcAG4AbABvAG8AawB1AHAAQQByAHIAYQB5ACwAIABCAFkAUgBPAFcAKABFAFgAUABBAE4ARAAoAEMASABPAE8AUwBFAEMATwBMAFMAKAByAGEAbgBnAGUALAAgAFMARQBRAFUARQBOAEMARQAoADEALAAgAGwAZQB2AGUAbABJAG4AZABlAHgAIAAtACAAMQApACkALAAgACwAIAAxADAALAAgAFwAIgBcACIAKQAsACAATABBAE0AQgBEAEEAKAByAG8AdwAsACAAVABFAFgAVABKAE8ASQBOACgAXwBzACwAIABGAEEATABTAEUALAAgAHIAbwB3ACkAKQApACwAXABuAHIAZQB0AHUAcgBuAFIAYQBuAGcAZQAsACAASQBOAEQARQBYACgAcgBhAG4AZwBlACwAIAAwACwAIABsAGUAdgBlAGwASQBuAGQAZQB4ACkALAAgAFwAbgByAGUAcwB1AGwAdAAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABsAG8AbwBrAHUAcAAxACkAIAAqACAAbABlAHYAZQBsAEkAbgBkAGUAeAAgAD0AIAAxACwAIAByAGUAdAB1AHIAbgBSAGEAbgBnAGUALAAgAFgATABPAE8ASwBVAFAAKABsAG8AbwBrAHUAcABWAGEAbAB1AGUALAAgAGwAbwBvAGsAdQBwAEEAcgByAGEAeQAsACAAcgBlAHQAdQByAG4AUgBhAG4AZwBlACkAOgBYAEwATwBPAEsAVQBQACgAbABvAG8AawB1AHAAVgBhAGwAdQBlACwAIABsAG8AbwBrAHUAcABBAHIAcgBhAHkALAAgAHIAZQB0AHUAcgBuAFIAYQBuAGcAZQAsACAALAAgACwAIAAtADEAKQApACwAXABuAHIAZQBzAHUAbAB0ACkAKQA7AFwAbgBcAG4ALwAvACAATQBhAHIAawAgAFAAcgBvAGMAdABvAHIAIABEAEQATABTAG8AcgB0AGUAcgAgAGYAdQBuAGMAdABpAG8AbgBcAG4AXABuAEQARABMAFMAbwByAHQAZQByAD0ATABBAE0AQgBEAEEAKABSAGEAbgBnAGUALABbAFMAbwByAHQATwByAGQAZQByAF0ALABTAE8AUgBUACgAUgBhAG4AZwBlACwAIABTAEUAUQBVAEUATgBDAEUAKAAsACAAQwBPAEwAVQBNAE4AUwAoAFIAYQBuAGcAZQApACkALAAgAFMAbwByAHQATwByAGQAZQByACkAKQA7AFwAbgBcAG4ALwAvACAARABvAHUAYgBsAGUAIABYAEwATwBPAEsAVQBQAFwAbgBcAG4AXwBmAEQAWAA9AEwAQQBNAEIARABBACgAdgBsAG8AbwBrAHUAcABfAHYAYQBsAHUAZQAsAHYAbABvAG8AawB1AHAAXwBhAHIAcgBhAHkALABoAGwAbwBvAGsAdQBwAF8AdgBhAGwAdQBlACwAaABsAG8AbwBrAHUAcABfAGEAcgByAGEAeQAsAHIAZQB0AHUAcgBuAF8AYQByAHIAYQB5ACwAWwBpAGYAXwBuAG8AdABfAGYAbwB1AG4AZABdACwAWwB2AG0AYQB0AGMAaABfAG0AbwBkAGUAXQAsAFsAdgBzAGUAYQByAGMAaABfAG0AbwBkAGUAXQAsAFsAaABtAGEAdABjAGgAXwBtAG8AZABlAF0ALABbAGgAcwBlAGEAcgBjAGgAXwBtAG8AZABlAF0ALAAgAEkARgBFAFIAUgBPAFIAKAAgAEkATgBEAEUAWAAoAHIAZQB0AHUAcgBuAF8AYQByAHIAYQB5ACwAWABNAEEAVABDAEgAKAB2AGwAbwBvAGsAdQBwAF8AdgBhAGwAdQBlACwAdgBsAG8AbwBrAHUAcABfAGEAcgByAGEAeQAsAHYAbQBhAHQAYwBoAF8AbQBvAGQAZQAsAHYAcwBlAGEAcgBjAGgAXwBtAG8AZABlACkALABYAE0AQQBUAEMASAAoAGgAbABvAG8AawB1AHAAXwB2AGEAbAB1AGUALABoAGwAbwBvAGsAdQBwAF8AYQByAHIAYQB5ACwAaABtAGEAdABjAGgAXwBtAG8AZABlACwAaABzAGUAYQByAGMAaABfAG0AbwBkAGUAKQApACwAIABJAEYAKABJAFMATwBNAGwAVABUAEUARAAoAGkAZgBfAG4AbwB0AF8AZgBvAHUAbgBkACkALABOAEEAKAApACwAaQBmAF8AbgBvAHQAXwBmAG8AdQBuAGQAKQApACkAOwBcAG4AXABuAC8ALwAgAFEAdQBhAHIAdABlAHIAIABmAHIAbwBtACAATQBvAG4AdABoACAAQQBiAGIAcgBlAHYAaQBhAHQAaQBvAG4AXABuAFwAbgBfAGYAUQA9AEwAQQBNAEIARABBACgAeAAsAFIATwBVAE4ARABVAFAAKABNAE8ATgBUAEgAKAAxACYAeAApAC8AMwAsADAAKQApADsAIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbACIAXwBmAEkAbgBkAGUAeAAiACwAIgBfAGYAUwBVAFAARQBSAFgATABPAE8ASwBVAFAAIgAsACIAXwBmAEkAbgB0AGUAcgBwACIALAAiAF8AZgBDAGgAYQByAEMAbwB1AG4AdAAiACwAIgBfAGYARABOACIALAAiAF8AZgBVAFAAIgAsACIAXwBmAEIAQwBBAFMAVAAiACwAIgBEAEQATAAiACwAIgBEAEQATABTAG8AcgB0AGUAcgAiACwAIgBfAGYARABYACIALAAiAF8AZgBRACIAXQAsACIAbABvAGMAYQBsAGUAIgA6AHsAIgBsAGkAcwB0AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAcgBvAHcAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBjAG8AbAB1AG0AbgBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAdABoAG8AdQBzAGEAbgBkAHMAUABvAHMAaQB0AGkAbwBuAHMAIgA6AFsAMwBdACwAIgBkAGUAYwBpAG0AYQBsAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiAC4AIgAsACIAZABhAHQAZQBPAHIAZABlAHIAIgA6ACIARABNAFkAIgAsACIAYwB1AHIAcgBlAG4AYwB5AFMAeQBtAGIAbwBsACIAOgAiACQAIgAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbABMAGUAYQBkACIAOgB0AHIAdQBlACwAIgBpAHMAQwB1AHIAcgBlAG4AYwB5AFMAZQBwAEIAeQBTAHAAYQBjAGUAIgA6AGYAYQBsAHMAZQAsACIAcgBvAHcATABlAHQAdABlAHIAIgA6ACIAUgAiACwAIgBjAG8AbAB1AG0AbgBMAGUAdAB0AGUAcgAiADoAIgBDACIALAAiAHIAYwBMAGUAZgB0AEIAcgBhAGMAawBlAHQAIgA6ACIAWwAiACwAIgByAGMAUgBpAGcAaAB0AEIAcgBhAGMAawBlAHQAIgA6ACIAXQAiACwAIgBzAHQAYQB0AGUAbQBlAG4AdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgA7ACIALAAiAGwAbwBjAGEAbABlAE4AYQBtAGUAIgA6ACIAZQBuAC0AdQBzACIAfQB9AA==</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30971B20-B398-44D5-A36C-AF779314A9EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
I was not able to use Pivotby to solve the problem
</commit_message>
<xml_diff>
--- a/CH-163 Custom Grouping.xlsx
+++ b/CH-163 Custom Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB81F83-8082-4142-8411-94FA128E6FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DC002C-938C-4FFA-8D23-31B9897AA9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,6 @@
     <definedName name="DDLSorter">_xlfn.LAMBDA(_xlpm.Range,_xlop.SortOrder, _xlfn._xlws.SORT(_xlpm.Range, _xlfn.SEQUENCE(, COLUMNS(_xlpm.Range)), _xlpm.SortOrder))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -75,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="22">
   <si>
     <t>Question</t>
   </si>
@@ -138,6 +137,9 @@
   </si>
   <si>
     <t>ROUNDUP(MONTH(--(1 &amp; C3:C39)) / 3, 0)</t>
+  </si>
+  <si>
+    <t>I don't see a way to use PIVOTBY to create the table we need.</t>
   </si>
 </sst>
 </file>
@@ -321,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -385,17 +387,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1058,17 +1063,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1"/>
-      <c r="G1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="G1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="K1" s="6" t="s">
         <v>19</v>
       </c>
@@ -1717,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F410690E-D8D2-49EA-83E7-40BEABC931DF}">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M59" sqref="M59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1734,17 +1739,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1"/>
-      <c r="G1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="G1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="K1" s="6" t="s">
         <v>19</v>
       </c>
@@ -2274,14 +2279,14 @@
       <c r="E21">
         <v>3</v>
       </c>
-      <c r="G21" s="4" cm="1">
+      <c r="G21" s="12" cm="1">
         <f t="array" ref="G21:I35">_xlfn.GROUPBY(_xlfn.HSTACK(B3:B39,E3:E39),D3:D39,_xleta.SUM,0,0)</f>
         <v>2020</v>
       </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21">
+      <c r="H21" s="13">
+        <v>1</v>
+      </c>
+      <c r="I21" s="14">
         <v>2255464</v>
       </c>
       <c r="K21" t="b" cm="1">
@@ -2309,13 +2314,13 @@
       <c r="E22">
         <v>4</v>
       </c>
-      <c r="G22" s="4">
-        <v>2020</v>
-      </c>
-      <c r="H22">
-        <v>2</v>
-      </c>
-      <c r="I22">
+      <c r="G22" s="15">
+        <v>2020</v>
+      </c>
+      <c r="H22" s="16">
+        <v>2</v>
+      </c>
+      <c r="I22" s="17">
         <v>1884296</v>
       </c>
       <c r="K22" t="b">
@@ -2343,13 +2348,13 @@
       <c r="E23">
         <v>4</v>
       </c>
-      <c r="G23" s="4">
-        <v>2020</v>
-      </c>
-      <c r="H23">
-        <v>3</v>
-      </c>
-      <c r="I23">
+      <c r="G23" s="18">
+        <v>2020</v>
+      </c>
+      <c r="H23" s="19">
+        <v>3</v>
+      </c>
+      <c r="I23" s="20">
         <v>2674392</v>
       </c>
       <c r="K23" t="b">
@@ -2375,13 +2380,13 @@
       <c r="E24">
         <v>1</v>
       </c>
-      <c r="G24" s="4">
-        <v>2020</v>
-      </c>
-      <c r="H24">
-        <v>4</v>
-      </c>
-      <c r="I24">
+      <c r="G24" s="21">
+        <v>2020</v>
+      </c>
+      <c r="H24" s="22">
+        <v>4</v>
+      </c>
+      <c r="I24" s="23">
         <v>2909572</v>
       </c>
       <c r="K24" t="b">
@@ -2407,13 +2412,13 @@
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="12">
         <v>2021</v>
       </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25">
+      <c r="H25" s="13">
+        <v>1</v>
+      </c>
+      <c r="I25" s="14">
         <v>2002380</v>
       </c>
       <c r="K25" t="b">
@@ -2439,13 +2444,13 @@
       <c r="E26">
         <v>1</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="15">
         <v>2021</v>
       </c>
-      <c r="H26">
-        <v>2</v>
-      </c>
-      <c r="I26">
+      <c r="H26" s="16">
+        <v>2</v>
+      </c>
+      <c r="I26" s="17">
         <v>3741940</v>
       </c>
       <c r="K26" t="b">
@@ -2471,13 +2476,13 @@
       <c r="E27">
         <v>2</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="18">
         <v>2021</v>
       </c>
-      <c r="H27">
-        <v>3</v>
-      </c>
-      <c r="I27">
+      <c r="H27" s="19">
+        <v>3</v>
+      </c>
+      <c r="I27" s="20">
         <v>3894246</v>
       </c>
       <c r="K27" t="b">
@@ -2503,13 +2508,13 @@
       <c r="E28">
         <v>2</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="21">
         <v>2021</v>
       </c>
-      <c r="H28">
-        <v>4</v>
-      </c>
-      <c r="I28">
+      <c r="H28" s="22">
+        <v>4</v>
+      </c>
+      <c r="I28" s="23">
         <v>2643503</v>
       </c>
       <c r="K28" t="b">
@@ -2535,13 +2540,13 @@
       <c r="E29">
         <v>2</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="12">
         <v>2022</v>
       </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="I29">
+      <c r="H29" s="13">
+        <v>1</v>
+      </c>
+      <c r="I29" s="14">
         <v>5857177</v>
       </c>
       <c r="K29" t="b">
@@ -2567,13 +2572,13 @@
       <c r="E30">
         <v>3</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="15">
         <v>2022</v>
       </c>
-      <c r="H30">
-        <v>2</v>
-      </c>
-      <c r="I30">
+      <c r="H30" s="16">
+        <v>2</v>
+      </c>
+      <c r="I30" s="17">
         <v>9621708</v>
       </c>
       <c r="K30" t="b">
@@ -2599,13 +2604,13 @@
       <c r="E31">
         <v>3</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="18">
         <v>2022</v>
       </c>
-      <c r="H31">
-        <v>3</v>
-      </c>
-      <c r="I31">
+      <c r="H31" s="19">
+        <v>3</v>
+      </c>
+      <c r="I31" s="20">
         <v>9939379</v>
       </c>
       <c r="K31" t="b">
@@ -2631,13 +2636,13 @@
       <c r="E32">
         <v>3</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="21">
         <v>2022</v>
       </c>
-      <c r="H32">
-        <v>4</v>
-      </c>
-      <c r="I32">
+      <c r="H32" s="22">
+        <v>4</v>
+      </c>
+      <c r="I32" s="23">
         <v>6377741</v>
       </c>
       <c r="K32" t="b">
@@ -2663,13 +2668,13 @@
       <c r="E33">
         <v>4</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="12">
         <v>2023</v>
       </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33">
+      <c r="H33" s="13">
+        <v>1</v>
+      </c>
+      <c r="I33" s="14">
         <v>9191668</v>
       </c>
       <c r="K33" t="b">
@@ -2695,13 +2700,13 @@
       <c r="E34">
         <v>4</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="15">
         <v>2023</v>
       </c>
-      <c r="H34">
-        <v>2</v>
-      </c>
-      <c r="I34">
+      <c r="H34" s="16">
+        <v>2</v>
+      </c>
+      <c r="I34" s="17">
         <v>12593541</v>
       </c>
       <c r="K34" t="b">
@@ -2727,13 +2732,13 @@
       <c r="E35">
         <v>1</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="18">
         <v>2023</v>
       </c>
-      <c r="H35">
-        <v>3</v>
-      </c>
-      <c r="I35">
+      <c r="H35" s="19">
+        <v>3</v>
+      </c>
+      <c r="I35" s="20">
         <v>6500793</v>
       </c>
       <c r="K35" t="b">
@@ -2787,7 +2792,7 @@
       <c r="E38">
         <v>2</v>
       </c>
-      <c r="G38" s="4" cm="1">
+      <c r="G38" s="12" cm="1">
         <f t="array" ref="G38:I52">_xlfn.LET(
     _xlpm.y, B3:B39,
     _xlpm.s, ROUNDUP(MONTH(--(1 &amp; C3:C39)) / 3, 0),
@@ -2795,10 +2800,10 @@
 )</f>
         <v>2020</v>
       </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-      <c r="I38">
+      <c r="H38" s="13">
+        <v>1</v>
+      </c>
+      <c r="I38" s="14">
         <v>2255464</v>
       </c>
       <c r="K38" t="b" cm="1">
@@ -2825,13 +2830,13 @@
       <c r="E39">
         <v>3</v>
       </c>
-      <c r="G39" s="4">
-        <v>2020</v>
-      </c>
-      <c r="H39">
-        <v>2</v>
-      </c>
-      <c r="I39">
+      <c r="G39" s="15">
+        <v>2020</v>
+      </c>
+      <c r="H39" s="16">
+        <v>2</v>
+      </c>
+      <c r="I39" s="17">
         <v>1884296</v>
       </c>
       <c r="K39" t="b">
@@ -2845,13 +2850,13 @@
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="G40" s="4">
-        <v>2020</v>
-      </c>
-      <c r="H40">
-        <v>3</v>
-      </c>
-      <c r="I40">
+      <c r="G40" s="18">
+        <v>2020</v>
+      </c>
+      <c r="H40" s="19">
+        <v>3</v>
+      </c>
+      <c r="I40" s="20">
         <v>2674392</v>
       </c>
       <c r="K40" t="b">
@@ -2865,13 +2870,13 @@
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="G41" s="4">
-        <v>2020</v>
-      </c>
-      <c r="H41">
-        <v>4</v>
-      </c>
-      <c r="I41">
+      <c r="G41" s="21">
+        <v>2020</v>
+      </c>
+      <c r="H41" s="22">
+        <v>4</v>
+      </c>
+      <c r="I41" s="23">
         <v>2909572</v>
       </c>
       <c r="K41" t="b">
@@ -2885,13 +2890,13 @@
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="G42" s="4">
+      <c r="G42" s="12">
         <v>2021</v>
       </c>
-      <c r="H42">
-        <v>1</v>
-      </c>
-      <c r="I42">
+      <c r="H42" s="13">
+        <v>1</v>
+      </c>
+      <c r="I42" s="14">
         <v>2002380</v>
       </c>
       <c r="K42" t="b">
@@ -2905,16 +2910,16 @@
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G43" s="15">
         <v>2021</v>
       </c>
-      <c r="H43">
-        <v>2</v>
-      </c>
-      <c r="I43">
+      <c r="H43" s="16">
+        <v>2</v>
+      </c>
+      <c r="I43" s="17">
         <v>3741940</v>
       </c>
       <c r="K43" t="b">
@@ -2928,13 +2933,13 @@
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="G44" s="4">
+      <c r="G44" s="18">
         <v>2021</v>
       </c>
-      <c r="H44">
-        <v>3</v>
-      </c>
-      <c r="I44">
+      <c r="H44" s="19">
+        <v>3</v>
+      </c>
+      <c r="I44" s="20">
         <v>3894246</v>
       </c>
       <c r="K44" t="b">
@@ -2968,13 +2973,13 @@
         <f t="array" ref="F45:F82">D45:D82=_xlfn.ANCHORARRAY(E45)</f>
         <v>1</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G45" s="21">
         <v>2021</v>
       </c>
-      <c r="H45">
-        <v>4</v>
-      </c>
-      <c r="I45">
+      <c r="H45" s="22">
+        <v>4</v>
+      </c>
+      <c r="I45" s="23">
         <v>2643503</v>
       </c>
       <c r="K45" t="b">
@@ -3004,13 +3009,13 @@
       <c r="F46" t="b">
         <v>1</v>
       </c>
-      <c r="G46" s="4">
+      <c r="G46" s="12">
         <v>2022</v>
       </c>
-      <c r="H46">
-        <v>1</v>
-      </c>
-      <c r="I46">
+      <c r="H46" s="13">
+        <v>1</v>
+      </c>
+      <c r="I46" s="14">
         <v>5857177</v>
       </c>
       <c r="K46" t="b">
@@ -3040,13 +3045,13 @@
       <c r="F47" t="b">
         <v>1</v>
       </c>
-      <c r="G47" s="4">
+      <c r="G47" s="15">
         <v>2022</v>
       </c>
-      <c r="H47">
-        <v>2</v>
-      </c>
-      <c r="I47">
+      <c r="H47" s="16">
+        <v>2</v>
+      </c>
+      <c r="I47" s="17">
         <v>9621708</v>
       </c>
       <c r="K47" t="b">
@@ -3076,13 +3081,13 @@
       <c r="F48" t="b">
         <v>1</v>
       </c>
-      <c r="G48" s="4">
+      <c r="G48" s="18">
         <v>2022</v>
       </c>
-      <c r="H48">
-        <v>3</v>
-      </c>
-      <c r="I48">
+      <c r="H48" s="19">
+        <v>3</v>
+      </c>
+      <c r="I48" s="20">
         <v>9939379</v>
       </c>
       <c r="K48" t="b">
@@ -3112,13 +3117,13 @@
       <c r="F49" t="b">
         <v>1</v>
       </c>
-      <c r="G49" s="4">
+      <c r="G49" s="21">
         <v>2022</v>
       </c>
-      <c r="H49">
-        <v>4</v>
-      </c>
-      <c r="I49">
+      <c r="H49" s="22">
+        <v>4</v>
+      </c>
+      <c r="I49" s="23">
         <v>6377741</v>
       </c>
       <c r="K49" t="b">
@@ -3148,13 +3153,13 @@
       <c r="F50" t="b">
         <v>1</v>
       </c>
-      <c r="G50" s="4">
+      <c r="G50" s="12">
         <v>2023</v>
       </c>
-      <c r="H50">
-        <v>1</v>
-      </c>
-      <c r="I50">
+      <c r="H50" s="13">
+        <v>1</v>
+      </c>
+      <c r="I50" s="14">
         <v>9191668</v>
       </c>
       <c r="K50" t="b">
@@ -3184,13 +3189,13 @@
       <c r="F51" t="b">
         <v>1</v>
       </c>
-      <c r="G51" s="4">
+      <c r="G51" s="15">
         <v>2023</v>
       </c>
-      <c r="H51">
-        <v>2</v>
-      </c>
-      <c r="I51">
+      <c r="H51" s="16">
+        <v>2</v>
+      </c>
+      <c r="I51" s="17">
         <v>12593541</v>
       </c>
       <c r="K51" t="b">
@@ -3220,13 +3225,13 @@
       <c r="F52" t="b">
         <v>1</v>
       </c>
-      <c r="G52" s="4">
+      <c r="G52" s="18">
         <v>2023</v>
       </c>
-      <c r="H52">
-        <v>3</v>
-      </c>
-      <c r="I52">
+      <c r="H52" s="19">
+        <v>3</v>
+      </c>
+      <c r="I52" s="20">
         <v>6500793</v>
       </c>
       <c r="K52" t="b">
@@ -3274,6 +3279,9 @@
       <c r="F54" t="b">
         <v>1</v>
       </c>
+      <c r="G54" s="29" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B55" s="3" t="str">
@@ -3292,6 +3300,25 @@
       <c r="F55" t="b">
         <v>1</v>
       </c>
+      <c r="G55" s="4" t="str" cm="1">
+        <f t="array" ref="G55:L72">_xlfn.PIVOTBY(_xlfn.HSTACK(B3:B39,E3:E39),E3:E39,D3:D39,_xleta.SUM,3,0,,0,,)</f>
+        <v/>
+      </c>
+      <c r="H55" t="str">
+        <v/>
+      </c>
+      <c r="I55" t="str">
+        <v>1</v>
+      </c>
+      <c r="J55" t="str">
+        <v/>
+      </c>
+      <c r="K55" t="str">
+        <v/>
+      </c>
+      <c r="L55" t="str">
+        <v/>
+      </c>
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B56" s="3" t="str">
@@ -3310,6 +3337,24 @@
       <c r="F56" t="b">
         <v>1</v>
       </c>
+      <c r="G56" s="4" t="str">
+        <v/>
+      </c>
+      <c r="H56" t="str">
+        <v/>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>2</v>
+      </c>
+      <c r="K56">
+        <v>3</v>
+      </c>
+      <c r="L56">
+        <v>4</v>
+      </c>
     </row>
     <row r="57" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B57" s="3" t="str">
@@ -3328,6 +3373,24 @@
       <c r="F57" t="b">
         <v>1</v>
       </c>
+      <c r="G57" s="4">
+        <v>2020</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>827837</v>
+      </c>
+      <c r="J57">
+        <v>827837</v>
+      </c>
+      <c r="K57">
+        <v>827837</v>
+      </c>
+      <c r="L57">
+        <v>827837</v>
+      </c>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B58" s="3" t="str">
@@ -3346,6 +3409,24 @@
       <c r="F58" t="b">
         <v>1</v>
       </c>
+      <c r="G58" s="4">
+        <v>2020</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>1427627</v>
+      </c>
+      <c r="J58" t="str">
+        <v/>
+      </c>
+      <c r="K58" t="str">
+        <v/>
+      </c>
+      <c r="L58" t="str">
+        <v/>
+      </c>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B59" s="3" t="str">
@@ -3364,6 +3445,24 @@
       <c r="F59" t="b">
         <v>1</v>
       </c>
+      <c r="G59" s="4">
+        <v>2020</v>
+      </c>
+      <c r="H59">
+        <v>2</v>
+      </c>
+      <c r="I59" t="str">
+        <v/>
+      </c>
+      <c r="J59">
+        <v>1884296</v>
+      </c>
+      <c r="K59" t="str">
+        <v/>
+      </c>
+      <c r="L59" t="str">
+        <v/>
+      </c>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B60" s="3" t="str">
@@ -3382,6 +3481,24 @@
       <c r="F60" t="b">
         <v>1</v>
       </c>
+      <c r="G60" s="4">
+        <v>2020</v>
+      </c>
+      <c r="H60">
+        <v>3</v>
+      </c>
+      <c r="I60" t="str">
+        <v/>
+      </c>
+      <c r="J60" t="str">
+        <v/>
+      </c>
+      <c r="K60">
+        <v>2674392</v>
+      </c>
+      <c r="L60" t="str">
+        <v/>
+      </c>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B61" s="3" t="str">
@@ -3400,6 +3517,24 @@
       <c r="F61" t="b">
         <v>1</v>
       </c>
+      <c r="G61" s="4">
+        <v>2020</v>
+      </c>
+      <c r="H61">
+        <v>4</v>
+      </c>
+      <c r="I61" t="str">
+        <v/>
+      </c>
+      <c r="J61" t="str">
+        <v/>
+      </c>
+      <c r="K61" t="str">
+        <v/>
+      </c>
+      <c r="L61">
+        <v>2909572</v>
+      </c>
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B62" s="3" t="str">
@@ -3418,6 +3553,24 @@
       <c r="F62" t="b">
         <v>1</v>
       </c>
+      <c r="G62" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>2002380</v>
+      </c>
+      <c r="J62" t="str">
+        <v/>
+      </c>
+      <c r="K62" t="str">
+        <v/>
+      </c>
+      <c r="L62" t="str">
+        <v/>
+      </c>
     </row>
     <row r="63" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B63" s="3" t="str">
@@ -3436,6 +3589,24 @@
       <c r="F63" t="b">
         <v>1</v>
       </c>
+      <c r="G63" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H63">
+        <v>2</v>
+      </c>
+      <c r="I63" t="str">
+        <v/>
+      </c>
+      <c r="J63">
+        <v>3741940</v>
+      </c>
+      <c r="K63" t="str">
+        <v/>
+      </c>
+      <c r="L63" t="str">
+        <v/>
+      </c>
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B64" s="3" t="str">
@@ -3454,8 +3625,26 @@
       <c r="F64" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G64" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H64">
+        <v>3</v>
+      </c>
+      <c r="I64" t="str">
+        <v/>
+      </c>
+      <c r="J64" t="str">
+        <v/>
+      </c>
+      <c r="K64">
+        <v>3894246</v>
+      </c>
+      <c r="L64" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B65" s="3" t="str">
         <v>1Nov</v>
       </c>
@@ -3472,8 +3661,26 @@
       <c r="F65" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G65" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H65">
+        <v>4</v>
+      </c>
+      <c r="I65" t="str">
+        <v/>
+      </c>
+      <c r="J65" t="str">
+        <v/>
+      </c>
+      <c r="K65" t="str">
+        <v/>
+      </c>
+      <c r="L65">
+        <v>2643503</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B66" s="3" t="str">
         <v>1Jan</v>
       </c>
@@ -3490,8 +3697,26 @@
       <c r="F66" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G66" s="4">
+        <v>2022</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>5857177</v>
+      </c>
+      <c r="J66" t="str">
+        <v/>
+      </c>
+      <c r="K66" t="str">
+        <v/>
+      </c>
+      <c r="L66" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B67" s="3" t="str">
         <v>1Feb</v>
       </c>
@@ -3508,8 +3733,26 @@
       <c r="F67" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G67" s="4">
+        <v>2022</v>
+      </c>
+      <c r="H67">
+        <v>2</v>
+      </c>
+      <c r="I67" t="str">
+        <v/>
+      </c>
+      <c r="J67">
+        <v>9621708</v>
+      </c>
+      <c r="K67" t="str">
+        <v/>
+      </c>
+      <c r="L67" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B68" s="3" t="str">
         <v>1Mar</v>
       </c>
@@ -3526,8 +3769,26 @@
       <c r="F68" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G68" s="4">
+        <v>2022</v>
+      </c>
+      <c r="H68">
+        <v>3</v>
+      </c>
+      <c r="I68" t="str">
+        <v/>
+      </c>
+      <c r="J68" t="str">
+        <v/>
+      </c>
+      <c r="K68">
+        <v>9939379</v>
+      </c>
+      <c r="L68" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B69" s="3" t="str">
         <v>1Apr</v>
       </c>
@@ -3544,8 +3805,26 @@
       <c r="F69" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G69" s="4">
+        <v>2022</v>
+      </c>
+      <c r="H69">
+        <v>4</v>
+      </c>
+      <c r="I69" t="str">
+        <v/>
+      </c>
+      <c r="J69" t="str">
+        <v/>
+      </c>
+      <c r="K69" t="str">
+        <v/>
+      </c>
+      <c r="L69">
+        <v>6377741</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B70" s="3" t="str">
         <v>1May</v>
       </c>
@@ -3562,8 +3841,26 @@
       <c r="F70" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G70" s="4">
+        <v>2023</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>9191668</v>
+      </c>
+      <c r="J70" t="str">
+        <v/>
+      </c>
+      <c r="K70" t="str">
+        <v/>
+      </c>
+      <c r="L70" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B71" s="3" t="str">
         <v>1Jun</v>
       </c>
@@ -3580,8 +3877,26 @@
       <c r="F71" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G71" s="4">
+        <v>2023</v>
+      </c>
+      <c r="H71">
+        <v>2</v>
+      </c>
+      <c r="I71" t="str">
+        <v/>
+      </c>
+      <c r="J71">
+        <v>12593541</v>
+      </c>
+      <c r="K71" t="str">
+        <v/>
+      </c>
+      <c r="L71" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B72" s="3" t="str">
         <v>1Jul</v>
       </c>
@@ -3598,8 +3913,26 @@
       <c r="F72" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G72" s="4">
+        <v>2023</v>
+      </c>
+      <c r="H72">
+        <v>3</v>
+      </c>
+      <c r="I72" t="str">
+        <v/>
+      </c>
+      <c r="J72" t="str">
+        <v/>
+      </c>
+      <c r="K72">
+        <v>6500793</v>
+      </c>
+      <c r="L72" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B73" s="3" t="str">
         <v>1Aug</v>
       </c>
@@ -3617,7 +3950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B74" s="3" t="str">
         <v>1Sep</v>
       </c>
@@ -3635,7 +3968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B75" s="3" t="str">
         <v>1Oct</v>
       </c>
@@ -3653,7 +3986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B76" s="3" t="str">
         <v>1Dec</v>
       </c>
@@ -3671,7 +4004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B77" s="3" t="str">
         <v>1Feb</v>
       </c>
@@ -3689,7 +4022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B78" s="3" t="str">
         <v>1Mar</v>
       </c>
@@ -3707,7 +4040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B79" s="3" t="str">
         <v>1Apr</v>
       </c>
@@ -3725,7 +4058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B80" s="3" t="str">
         <v>1Jun</v>
       </c>
@@ -3767,7 +4100,7 @@
       </c>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B84" s="28"/>
+      <c r="B84" s="26"/>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B85" s="3" cm="1">

</xml_diff>